<commit_message>
Add new summary & Draft file
</commit_message>
<xml_diff>
--- a/data/Draft_3rdparty.xlsx
+++ b/data/Draft_3rdparty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Magang ITM Tbk\Automation\SystemAutomation_WeeklyReport\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4B6986-9C32-4994-96A1-D5231ABD2557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E587408E-D7C5-4F26-BFD0-69AF4ECBFEDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="18252" windowHeight="6696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3rd Party" sheetId="1" r:id="rId1"/>
@@ -1359,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="69" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1549,7 +1549,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="12">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="F11" s="12">
         <v>0</v>
@@ -1566,7 +1566,7 @@
         <v>6</v>
       </c>
       <c r="E12" s="12">
-        <v>0</v>
+        <v>45000</v>
       </c>
       <c r="F12" s="12">
         <v>0</v>
@@ -1583,10 +1583,10 @@
         <v>6</v>
       </c>
       <c r="E13" s="12">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="F13" s="12">
-        <v>0</v>
+        <v>30109.16</v>
       </c>
     </row>
     <row r="14" spans="2:12">
@@ -1600,10 +1600,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="12">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="F14" s="12">
-        <v>0</v>
+        <v>22742</v>
       </c>
     </row>
     <row r="15" spans="2:12">
@@ -1957,10 +1957,10 @@
         <v>9</v>
       </c>
       <c r="E35" s="12">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="F35" s="12">
-        <v>0</v>
+        <v>59600</v>
       </c>
     </row>
     <row r="36" spans="2:6">
@@ -1974,10 +1974,10 @@
         <v>9</v>
       </c>
       <c r="E36" s="12">
-        <v>0</v>
+        <v>52500</v>
       </c>
       <c r="F36" s="12">
-        <v>0</v>
+        <v>52500</v>
       </c>
     </row>
     <row r="37" spans="2:6">
@@ -1991,10 +1991,10 @@
         <v>9</v>
       </c>
       <c r="E37" s="12">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="F37" s="12">
-        <v>0</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="38" spans="2:6">
@@ -2008,10 +2008,10 @@
         <v>9</v>
       </c>
       <c r="E38" s="12">
-        <v>0</v>
+        <v>67500</v>
       </c>
       <c r="F38" s="12">
-        <v>0</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="39" spans="2:6">
@@ -2161,10 +2161,10 @@
         <v>10</v>
       </c>
       <c r="E47" s="12">
-        <v>0</v>
+        <v>45000</v>
       </c>
       <c r="F47" s="12">
-        <v>0</v>
+        <v>22500</v>
       </c>
     </row>
     <row r="48" spans="2:6">
@@ -2178,10 +2178,10 @@
         <v>10</v>
       </c>
       <c r="E48" s="12">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="F48" s="12">
-        <v>0</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="49" spans="2:6">
@@ -2195,10 +2195,10 @@
         <v>10</v>
       </c>
       <c r="E49" s="12">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="F49" s="12">
-        <v>0</v>
+        <v>29900</v>
       </c>
     </row>
     <row r="50" spans="2:6">
@@ -2212,10 +2212,10 @@
         <v>10</v>
       </c>
       <c r="E50" s="12">
-        <v>0</v>
+        <v>45000</v>
       </c>
       <c r="F50" s="12">
-        <v>0</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="51" spans="2:6">
@@ -2365,10 +2365,10 @@
         <v>11</v>
       </c>
       <c r="E59" s="12">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="F59" s="12">
-        <v>0</v>
+        <v>89457.65</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2382,10 +2382,10 @@
         <v>11</v>
       </c>
       <c r="E60" s="12">
-        <v>0</v>
+        <v>37500</v>
       </c>
       <c r="F60" s="12">
-        <v>0</v>
+        <v>15007.91</v>
       </c>
     </row>
     <row r="61" spans="2:6">
@@ -2399,10 +2399,10 @@
         <v>11</v>
       </c>
       <c r="E61" s="12">
-        <v>0</v>
+        <v>22500</v>
       </c>
       <c r="F61" s="12">
-        <v>0</v>
+        <v>15008.51</v>
       </c>
     </row>
     <row r="62" spans="2:6">
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="12">
-        <v>0</v>
+        <v>37115</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2569,10 +2569,10 @@
         <v>13</v>
       </c>
       <c r="E71" s="12">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="F71" s="12">
-        <v>0</v>
+        <v>14850</v>
       </c>
     </row>
     <row r="72" spans="2:6">
@@ -2586,10 +2586,10 @@
         <v>13</v>
       </c>
       <c r="E72" s="12">
-        <v>0</v>
+        <v>22500</v>
       </c>
       <c r="F72" s="12">
-        <v>0</v>
+        <v>29602</v>
       </c>
     </row>
     <row r="73" spans="2:6">
@@ -2603,10 +2603,10 @@
         <v>13</v>
       </c>
       <c r="E73" s="12">
-        <v>0</v>
+        <v>22500</v>
       </c>
       <c r="F73" s="12">
-        <v>0</v>
+        <v>29641</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -2620,10 +2620,10 @@
         <v>13</v>
       </c>
       <c r="E74" s="12">
-        <v>0</v>
+        <v>22500</v>
       </c>
       <c r="F74" s="12">
-        <v>0</v>
+        <v>20071</v>
       </c>
     </row>
     <row r="75" spans="2:6">
@@ -2759,6 +2759,7 @@
         <v>21200</v>
       </c>
       <c r="F82" s="12">
+        <f>20946-5300</f>
         <v>15646</v>
       </c>
     </row>
@@ -2773,10 +2774,10 @@
         <v>14</v>
       </c>
       <c r="E83" s="12">
-        <v>0</v>
+        <v>21200</v>
       </c>
       <c r="F83" s="12">
-        <v>0</v>
+        <v>15831</v>
       </c>
     </row>
     <row r="84" spans="2:6">
@@ -2790,10 +2791,10 @@
         <v>14</v>
       </c>
       <c r="E84" s="12">
-        <v>0</v>
+        <v>21200</v>
       </c>
       <c r="F84" s="12">
-        <v>0</v>
+        <v>15924</v>
       </c>
     </row>
     <row r="85" spans="2:6">
@@ -2807,10 +2808,10 @@
         <v>14</v>
       </c>
       <c r="E85" s="12">
-        <v>0</v>
+        <v>15900</v>
       </c>
       <c r="F85" s="12">
-        <v>0</v>
+        <v>15376</v>
       </c>
     </row>
     <row r="86" spans="2:6">
@@ -2824,10 +2825,10 @@
         <v>14</v>
       </c>
       <c r="E86" s="12">
-        <v>0</v>
+        <v>21200</v>
       </c>
       <c r="F86" s="12">
-        <v>0</v>
+        <v>10446</v>
       </c>
     </row>
     <row r="87" spans="2:6">
@@ -2963,6 +2964,7 @@
         <v>21200</v>
       </c>
       <c r="F94" s="12">
+        <f>21225-5300</f>
         <v>15925</v>
       </c>
     </row>
@@ -2977,10 +2979,10 @@
         <v>15</v>
       </c>
       <c r="E95" s="12">
-        <v>0</v>
+        <v>21200</v>
       </c>
       <c r="F95" s="12">
-        <v>0</v>
+        <v>26050</v>
       </c>
     </row>
     <row r="96" spans="2:6">
@@ -2994,10 +2996,10 @@
         <v>15</v>
       </c>
       <c r="E96" s="12">
-        <v>0</v>
+        <v>15900</v>
       </c>
       <c r="F96" s="12">
-        <v>0</v>
+        <v>20919</v>
       </c>
     </row>
     <row r="97" spans="2:6">
@@ -3011,10 +3013,10 @@
         <v>15</v>
       </c>
       <c r="E97" s="12">
-        <v>0</v>
+        <v>21200</v>
       </c>
       <c r="F97" s="12">
-        <v>0</v>
+        <v>20989</v>
       </c>
     </row>
     <row r="98" spans="2:6">
@@ -3028,10 +3030,10 @@
         <v>15</v>
       </c>
       <c r="E98" s="12">
-        <v>0</v>
+        <v>15900</v>
       </c>
       <c r="F98" s="12">
-        <v>0</v>
+        <v>15778</v>
       </c>
     </row>
     <row r="99" spans="2:6">
@@ -3181,10 +3183,10 @@
         <v>16</v>
       </c>
       <c r="E107" s="12">
-        <v>0</v>
+        <v>10600</v>
       </c>
       <c r="F107" s="12">
-        <v>0</v>
+        <v>10538</v>
       </c>
     </row>
     <row r="108" spans="2:6">
@@ -3198,10 +3200,10 @@
         <v>16</v>
       </c>
       <c r="E108" s="12">
-        <v>0</v>
+        <v>5300</v>
       </c>
       <c r="F108" s="12">
-        <v>0</v>
+        <v>15493</v>
       </c>
     </row>
     <row r="109" spans="2:6">
@@ -3215,10 +3217,10 @@
         <v>16</v>
       </c>
       <c r="E109" s="12">
-        <v>0</v>
+        <v>10600</v>
       </c>
       <c r="F109" s="12">
-        <v>0</v>
+        <v>5280</v>
       </c>
     </row>
     <row r="110" spans="2:6">
@@ -3232,10 +3234,10 @@
         <v>16</v>
       </c>
       <c r="E110" s="12">
-        <v>0</v>
+        <v>15900</v>
       </c>
       <c r="F110" s="12">
-        <v>0</v>
+        <v>10355</v>
       </c>
     </row>
     <row r="111" spans="2:6">
@@ -3385,10 +3387,10 @@
         <v>18</v>
       </c>
       <c r="E119" s="12">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="F119" s="12">
-        <v>0</v>
+        <v>7201</v>
       </c>
     </row>
     <row r="120" spans="2:6">
@@ -3402,7 +3404,7 @@
         <v>18</v>
       </c>
       <c r="E120" s="12">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="F120" s="12">
         <v>0</v>
@@ -3419,10 +3421,10 @@
         <v>18</v>
       </c>
       <c r="E121" s="12">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="F121" s="12">
-        <v>0</v>
+        <v>30009</v>
       </c>
     </row>
     <row r="122" spans="2:6">
@@ -3436,10 +3438,10 @@
         <v>18</v>
       </c>
       <c r="E122" s="12">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="F122" s="12">
-        <v>0</v>
+        <v>24811</v>
       </c>
     </row>
     <row r="123" spans="2:6">
@@ -3575,7 +3577,7 @@
         <v>31800</v>
       </c>
       <c r="F130" s="12">
-        <v>14823.35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="2:6">
@@ -3589,10 +3591,10 @@
         <v>19</v>
       </c>
       <c r="E131" s="12">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="F131" s="12">
-        <v>0</v>
+        <v>45555</v>
       </c>
     </row>
     <row r="132" spans="2:6">
@@ -3606,10 +3608,10 @@
         <v>19</v>
       </c>
       <c r="E132" s="12">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="F132" s="12">
-        <v>0</v>
+        <v>55551.540000000008</v>
       </c>
     </row>
     <row r="133" spans="2:6">
@@ -3623,10 +3625,10 @@
         <v>19</v>
       </c>
       <c r="E133" s="12">
-        <v>0</v>
+        <v>55300</v>
       </c>
       <c r="F133" s="12">
-        <v>0</v>
+        <v>70751.64</v>
       </c>
     </row>
     <row r="134" spans="2:6">
@@ -3640,10 +3642,10 @@
         <v>19</v>
       </c>
       <c r="E134" s="12">
-        <v>0</v>
+        <v>82500</v>
       </c>
       <c r="F134" s="12">
-        <v>0</v>
+        <v>37311</v>
       </c>
     </row>
     <row r="135" spans="2:6">
@@ -3793,10 +3795,10 @@
         <v>20</v>
       </c>
       <c r="E143" s="12">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="F143" s="12">
-        <v>0</v>
+        <v>5340</v>
       </c>
     </row>
     <row r="144" spans="2:6">
@@ -3810,10 +3812,10 @@
         <v>20</v>
       </c>
       <c r="E144" s="12">
-        <v>0</v>
+        <v>10600</v>
       </c>
       <c r="F144" s="12">
-        <v>0</v>
+        <v>5305</v>
       </c>
     </row>
     <row r="145" spans="2:6">
@@ -4405,7 +4407,7 @@
         <v>24</v>
       </c>
       <c r="E179" s="12">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="F179" s="12">
         <v>0</v>
@@ -4439,7 +4441,7 @@
         <v>24</v>
       </c>
       <c r="E181" s="12">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="F181" s="12">
         <v>0</v>
@@ -4456,10 +4458,10 @@
         <v>24</v>
       </c>
       <c r="E182" s="12">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="F182" s="12">
-        <v>0</v>
+        <v>15368</v>
       </c>
     </row>
     <row r="183" spans="2:6">
@@ -5017,7 +5019,7 @@
         <v>27</v>
       </c>
       <c r="E215" s="12">
-        <v>0</v>
+        <v>22500</v>
       </c>
       <c r="F215" s="12">
         <v>0</v>
@@ -5034,10 +5036,10 @@
         <v>27</v>
       </c>
       <c r="E216" s="12">
-        <v>0</v>
+        <v>52500</v>
       </c>
       <c r="F216" s="12">
-        <v>0</v>
+        <v>7601</v>
       </c>
     </row>
     <row r="217" spans="2:6">
@@ -5051,10 +5053,10 @@
         <v>27</v>
       </c>
       <c r="E217" s="12">
-        <v>0</v>
+        <v>52500</v>
       </c>
       <c r="F217" s="12">
-        <v>0</v>
+        <v>7600</v>
       </c>
     </row>
     <row r="218" spans="2:6">
@@ -5068,10 +5070,10 @@
         <v>27</v>
       </c>
       <c r="E218" s="12">
-        <v>0</v>
+        <v>45000</v>
       </c>
       <c r="F218" s="12">
-        <v>0</v>
+        <v>45227</v>
       </c>
     </row>
     <row r="219" spans="2:6">
@@ -5700,7 +5702,7 @@
   <dimension ref="B2:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5763,7 +5765,7 @@
         <v>45566</v>
       </c>
     </row>
-    <row r="13" spans="2:2" ht="31.2" customHeight="1">
+    <row r="13" spans="2:2" ht="18.600000000000001" customHeight="1">
       <c r="B13" s="7">
         <v>45597</v>
       </c>
@@ -5785,8 +5787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:L242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H154" sqref="H154"/>
+    <sheetView topLeftCell="A9" zoomScale="64" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>